<commit_message>
Convert to cloudbite backend
</commit_message>
<xml_diff>
--- a/SeleniumTests/TestCaseTemplate.xlsx
+++ b/SeleniumTests/TestCaseTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\e-invoice\SeleniumTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733BE091-3F14-4326-AA52-CCB83353AB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6EC40F-6A7B-4230-A8B7-A02E6805052F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{7A1E2798-C7FD-4832-92CA-34B758243353}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7A1E2798-C7FD-4832-92CA-34B758243353}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case" sheetId="1" r:id="rId1"/>
@@ -152,10 +152,6 @@
     <t>TEST DATA</t>
   </si>
   <si>
-    <t>STATUS 
-(PASS / FAILED)</t>
-  </si>
-  <si>
     <t>REMARK</t>
   </si>
   <si>
@@ -168,8 +164,12 @@
     <t>Alan Ong</t>
   </si>
   <si>
-    <t>Ong Ze Liang
+    <t>Lucas
 Fahmy</t>
+  </si>
+  <si>
+    <t>STATUS 
+(Passed / Failed)</t>
   </si>
 </sst>
 </file>
@@ -480,15 +480,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -497,36 +527,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -557,9 +557,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
+      <xdr:colOff>739140</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>450233</xdr:rowOff>
+      <xdr:rowOff>446423</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -914,7 +914,7 @@
   <dimension ref="A1:O200"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G20" sqref="G20:G200 I20:I200 K20:K200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -934,13 +934,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="47"/>
-      <c r="B1" s="47"/>
+      <c r="A1" s="39"/>
+      <c r="B1" s="39"/>
       <c r="C1" s="28" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" s="30" t="s">
         <v>1</v>
@@ -957,66 +957,66 @@
       <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="28" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="29"/>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="40" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="43"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="39"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="46"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="47"/>
-      <c r="B3" s="47"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="31" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="29"/>
-      <c r="E3" s="49"/>
+      <c r="E3" s="41"/>
       <c r="F3" s="44"/>
       <c r="G3" s="44"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="39"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="46"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="47"/>
-      <c r="B4" s="47"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="28" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="29"/>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="51" t="s">
-        <v>37</v>
+      <c r="F4" s="45" t="s">
+        <v>36</v>
       </c>
       <c r="G4" s="43"/>
       <c r="H4" s="43"/>
-      <c r="I4" s="39"/>
+      <c r="I4" s="46"/>
     </row>
     <row r="5" spans="1:15" ht="141" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47"/>
-      <c r="B5" s="47"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="28" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="27"/>
-      <c r="E5" s="49"/>
+      <c r="E5" s="41"/>
       <c r="F5" s="44"/>
       <c r="G5" s="44"/>
       <c r="H5" s="44"/>
-      <c r="I5" s="39"/>
+      <c r="I5" s="46"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="47"/>
-      <c r="B6" s="47"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="31" t="s">
         <v>11</v>
       </c>
@@ -1025,19 +1025,19 @@
         <v>12</v>
       </c>
       <c r="F6" s="43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" s="43"/>
       <c r="H6" s="43"/>
-      <c r="I6" s="39"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50"/>
-      <c r="N6" s="50"/>
-      <c r="O6" s="50"/>
+      <c r="I6" s="46"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="42"/>
+      <c r="O6" s="42"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="47"/>
-      <c r="B7" s="47"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="39"/>
       <c r="C7" s="28" t="s">
         <v>13</v>
       </c>
@@ -1046,15 +1046,15 @@
       <c r="F7" s="44"/>
       <c r="G7" s="44"/>
       <c r="H7" s="44"/>
-      <c r="I7" s="39"/>
+      <c r="I7" s="46"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="47"/>
-      <c r="B8" s="47"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="28" t="s">
         <v>14</v>
       </c>
@@ -1072,8 +1072,8 @@
       <c r="O8" s="10"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="47"/>
-      <c r="B9" s="47"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="28" t="s">
         <v>16</v>
       </c>
@@ -1092,13 +1092,13 @@
       <c r="L10" s="9"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="42"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="52"/>
       <c r="F11" s="34"/>
       <c r="G11" s="35"/>
     </row>
@@ -1113,7 +1113,7 @@
         <v>19</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>20</v>
@@ -1210,18 +1210,18 @@
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G18" s="45" t="s">
+      <c r="G18" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="46"/>
-      <c r="I18" s="45" t="s">
+      <c r="H18" s="38"/>
+      <c r="I18" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="46"/>
-      <c r="K18" s="45" t="s">
+      <c r="J18" s="38"/>
+      <c r="K18" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="L18" s="46"/>
+      <c r="L18" s="38"/>
     </row>
     <row r="19" spans="1:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
@@ -1243,22 +1243,22 @@
         <v>31</v>
       </c>
       <c r="G19" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="H19" s="19" t="s">
-        <v>33</v>
-      </c>
       <c r="I19" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="J19" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="J19" s="19" t="s">
-        <v>33</v>
-      </c>
       <c r="K19" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="L19" s="19" t="s">
         <v>32</v>
-      </c>
-      <c r="L19" s="19" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.3">
@@ -3797,6 +3797,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="I18:J18"/>
     <mergeCell ref="K18:L18"/>
@@ -3813,17 +3820,10 @@
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G20:G200 I20:I200 K20:K200" xr:uid="{71CD85F8-624E-4B0E-B311-937AD723C12C}">
-      <formula1>"PASS,FAILED,NOT EXECUTED"</formula1>
+      <formula1>"Passed,Failed,NOT EXECUTED"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Complete Store Module (Positive)
</commit_message>
<xml_diff>
--- a/SeleniumTests/TestCaseTemplate.xlsx
+++ b/SeleniumTests/TestCaseTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\e-invoice\SeleniumTests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cloudbite\SeleniumTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6EC40F-6A7B-4230-A8B7-A02E6805052F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9944A3-E7D5-438E-8AB2-05BBA9003A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7A1E2798-C7FD-4832-92CA-34B758243353}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{7A1E2798-C7FD-4832-92CA-34B758243353}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t xml:space="preserve">Project: </t>
   </si>
@@ -159,13 +159,6 @@
   </si>
   <si>
     <t>E-Invoice Portal</t>
-  </si>
-  <si>
-    <t>Alan Ong</t>
-  </si>
-  <si>
-    <t>Lucas
-Fahmy</t>
   </si>
   <si>
     <t>STATUS 
@@ -914,7 +907,7 @@
   <dimension ref="A1:O200"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20:G200 I20:I200 K20:K200"/>
+      <selection activeCell="F6" sqref="F6:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -994,9 +987,7 @@
       <c r="E4" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="45" t="s">
-        <v>36</v>
-      </c>
+      <c r="F4" s="45"/>
       <c r="G4" s="43"/>
       <c r="H4" s="43"/>
       <c r="I4" s="46"/>
@@ -1024,9 +1015,7 @@
       <c r="E6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="43" t="s">
-        <v>35</v>
-      </c>
+      <c r="F6" s="43"/>
       <c r="G6" s="43"/>
       <c r="H6" s="43"/>
       <c r="I6" s="46"/>
@@ -1243,19 +1232,19 @@
         <v>31</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H19" s="19" t="s">
         <v>32</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J19" s="19" t="s">
         <v>32</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L19" s="19" t="s">
         <v>32</v>

</xml_diff>